<commit_message>
FEAT: plot color and shape changed
</commit_message>
<xml_diff>
--- a/pll_data.xlsx
+++ b/pll_data.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETH\PhD\PLL_survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB1AE20-A39B-4C04-9A0C-F6CD7E7246A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8275D3EE-69D1-46E1-B89F-1D390FE884CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC291710-661A-4111-9329-6CD384A593DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
     <sheet name="Republished Papers" sheetId="2" r:id="rId2"/>
+    <sheet name="Item guide" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>Tags</t>
   </si>
   <si>
     <t>A Low-Jitter and Compact-Area Fractional-N Digital PLL With Fast Multi-Variable Calibration Using the Recursive Least-Squares Algorithm</t>
@@ -553,9 +551,6 @@
     <t>Ours</t>
   </si>
   <si>
-    <t>Put your results here</t>
-  </si>
-  <si>
     <t>Fractional-N Digital MDLL With Injection-Error Scrambling and Calibration</t>
   </si>
   <si>
@@ -919,12 +914,48 @@
   <si>
     <t>Plot</t>
   </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Jitter</t>
+  </si>
+  <si>
+    <t>Tags (optional)</t>
+  </si>
+  <si>
+    <t>TDC</t>
+  </si>
+  <si>
+    <t>BB/TDC</t>
+  </si>
+  <si>
+    <t>PhaseDetector</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Leave FracSpur column empty if PLL is integer-N.</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>JSSC'2-</t>
+  </si>
+  <si>
+    <t>Designate without date if the item is eary access.</t>
+  </si>
+  <si>
+    <t>Put your own results here for comparison</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1059,8 +1090,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1240,6 +1293,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1357,7 +1422,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1400,14 +1465,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1441,6 +1511,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1781,27 +1852,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB6C843-7974-497E-9814-12CC7D1E0204}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1810,1447 +1882,1782 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" t="s">
         <v>120</v>
       </c>
-      <c r="G1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>121</v>
       </c>
-      <c r="I1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2">
         <v>-255</v>
       </c>
       <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
         <v>-70</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.6</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>65</v>
       </c>
-      <c r="I2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J2" t="s">
-        <v>129</v>
-      </c>
       <c r="K2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>210</v>
+      </c>
+      <c r="M2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="E3">
         <v>-249.1</v>
       </c>
       <c r="F3">
+        <v>15.7</v>
+      </c>
+      <c r="G3">
+        <v>88</v>
+      </c>
+      <c r="H3">
         <v>-68</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.12</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>40</v>
       </c>
-      <c r="I3" t="s">
-        <v>124</v>
-      </c>
-      <c r="J3" t="s">
-        <v>129</v>
-      </c>
       <c r="K3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" t="s">
+        <v>211</v>
+      </c>
+      <c r="M3" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4">
         <v>-253.5</v>
       </c>
       <c r="F4">
+        <v>17.5</v>
+      </c>
+      <c r="G4">
+        <v>57.3</v>
+      </c>
+      <c r="H4">
         <v>-63.4</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.21</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J4" t="s">
-        <v>129</v>
-      </c>
       <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" t="s">
+        <v>213</v>
+      </c>
+      <c r="M4" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5">
         <v>-251</v>
       </c>
       <c r="F5">
+        <v>7.3</v>
+      </c>
+      <c r="G5">
+        <v>104</v>
+      </c>
+      <c r="H5">
         <v>-58</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.21</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>65</v>
       </c>
-      <c r="I5" t="s">
-        <v>124</v>
-      </c>
-      <c r="J5" t="s">
-        <v>129</v>
-      </c>
       <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" t="s">
+        <v>215</v>
+      </c>
+      <c r="M5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
         <v>15</v>
       </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="E6">
         <v>-242.9</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
+        <v>14.2</v>
+      </c>
+      <c r="G6">
+        <v>191</v>
+      </c>
+      <c r="H6" s="1">
         <v>-52.7</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0.48</v>
       </c>
-      <c r="H6" s="1">
+      <c r="J6" s="1">
         <v>65</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" t="s">
         <v>19</v>
       </c>
-      <c r="L6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="E7">
         <v>-247.4</v>
       </c>
       <c r="F7">
+        <v>8.89</v>
+      </c>
+      <c r="G7">
+        <v>143.69999999999999</v>
+      </c>
+      <c r="H7">
         <v>-62.1</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>0.23</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>65</v>
       </c>
-      <c r="I7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" t="s">
-        <v>129</v>
-      </c>
       <c r="K7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" t="s">
+        <v>213</v>
+      </c>
+      <c r="M7" t="s">
+        <v>128</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
         <v>23</v>
       </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E8">
         <v>-246.2</v>
       </c>
       <c r="F8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G8">
+        <v>233</v>
+      </c>
+      <c r="H8">
         <v>-60.6</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>0.31</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>40</v>
       </c>
-      <c r="I8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J8" t="s">
-        <v>129</v>
-      </c>
       <c r="K8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" t="s">
+        <v>210</v>
+      </c>
+      <c r="M8" t="s">
+        <v>128</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
         <v>27</v>
       </c>
-      <c r="L8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9">
         <v>-230.6</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
+        <v>13.56</v>
+      </c>
+      <c r="G9">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="1">
         <v>-67</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <v>0.23</v>
       </c>
-      <c r="H9" s="1">
+      <c r="J9" s="1">
         <v>65</v>
       </c>
-      <c r="I9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J9" t="s">
-        <v>128</v>
-      </c>
       <c r="K9" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="L9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M9" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10">
         <v>-250</v>
       </c>
       <c r="F10">
+        <v>17.2</v>
+      </c>
+      <c r="G10">
+        <v>77</v>
+      </c>
+      <c r="H10">
         <v>-71.900000000000006</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>0.33</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>28</v>
       </c>
-      <c r="I10" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" t="s">
-        <v>129</v>
-      </c>
       <c r="K10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" t="s">
+        <v>213</v>
+      </c>
+      <c r="M10" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" t="s">
         <v>31</v>
       </c>
-      <c r="L10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11">
         <v>-251.7</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>59.78</v>
+      </c>
+      <c r="H11" s="1">
         <v>-58.7</v>
       </c>
-      <c r="G11" s="1">
+      <c r="I11" s="1">
         <v>0.23</v>
       </c>
-      <c r="H11" s="1">
+      <c r="J11" s="1">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
-        <v>124</v>
-      </c>
-      <c r="J11" t="s">
-        <v>129</v>
-      </c>
       <c r="K11" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="L11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M11" t="s">
+        <v>128</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="O11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12">
         <v>-250.6</v>
       </c>
       <c r="F12">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G12">
+        <v>135</v>
+      </c>
+      <c r="H12">
         <v>-57</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>0.38</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>65</v>
       </c>
-      <c r="I12" t="s">
-        <v>124</v>
-      </c>
-      <c r="J12" t="s">
-        <v>129</v>
-      </c>
       <c r="K12" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="L12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13">
         <v>-249.4</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
+        <v>3.5</v>
+      </c>
+      <c r="G13">
+        <v>182</v>
+      </c>
+      <c r="H13" s="1">
         <v>-59</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
         <v>0.31</v>
       </c>
-      <c r="H13" s="1">
+      <c r="J13" s="1">
         <v>40</v>
       </c>
-      <c r="I13" t="s">
-        <v>123</v>
-      </c>
-      <c r="J13" t="s">
-        <v>129</v>
-      </c>
       <c r="K13" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="L13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M13" t="s">
+        <v>128</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="O13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E14">
         <v>-248.7</v>
       </c>
       <c r="F14">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <v>72</v>
+      </c>
+      <c r="H14">
         <v>-59.7</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>0.47</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>28</v>
       </c>
-      <c r="I14" t="s">
-        <v>124</v>
-      </c>
-      <c r="J14" t="s">
-        <v>129</v>
-      </c>
       <c r="K14" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="L14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M14" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E15" s="1">
         <v>-251.5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
+        <v>10.8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>79.7</v>
+      </c>
+      <c r="H15">
         <v>-51.1</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>0.21</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>28</v>
       </c>
-      <c r="I15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J15" t="s">
-        <v>129</v>
-      </c>
       <c r="K15" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" t="s">
+        <v>213</v>
+      </c>
+      <c r="M15" t="s">
+        <v>128</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15" t="s">
         <v>35</v>
       </c>
-      <c r="L15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16">
         <v>-224.8</v>
       </c>
       <c r="F16">
+        <v>11.95</v>
+      </c>
+      <c r="G16">
+        <v>1670</v>
+      </c>
+      <c r="H16">
         <v>-52</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>0.18</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>65</v>
       </c>
-      <c r="I16" t="s">
-        <v>126</v>
-      </c>
-      <c r="J16" t="s">
-        <v>128</v>
-      </c>
       <c r="K16" t="s">
+        <v>125</v>
+      </c>
+      <c r="L16" t="s">
+        <v>210</v>
+      </c>
+      <c r="M16" t="s">
+        <v>127</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" t="s">
         <v>39</v>
       </c>
-      <c r="L16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17">
         <v>-242.3</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
+        <v>3.25</v>
+      </c>
+      <c r="G17">
+        <v>428</v>
+      </c>
+      <c r="H17" s="1">
         <v>-55</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>0.39</v>
       </c>
-      <c r="H17" s="1">
+      <c r="J17" s="1">
         <v>40</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="K17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" t="s">
         <v>43</v>
       </c>
-      <c r="L17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18">
         <v>-247.5</v>
       </c>
       <c r="F18">
+        <v>11.7</v>
+      </c>
+      <c r="G18">
+        <v>405</v>
+      </c>
+      <c r="H18">
         <v>-50</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>0.61</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>65</v>
       </c>
-      <c r="I18" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" t="s">
-        <v>128</v>
-      </c>
       <c r="K18" t="s">
+        <v>122</v>
+      </c>
+      <c r="L18" t="s">
+        <v>210</v>
+      </c>
+      <c r="M18" t="s">
+        <v>127</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" t="s">
         <v>47</v>
       </c>
-      <c r="L18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19">
         <v>-239.1</v>
       </c>
       <c r="F19">
+        <v>9.27</v>
+      </c>
+      <c r="G19">
+        <v>365</v>
+      </c>
+      <c r="H19">
         <v>-63</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>65</v>
       </c>
-      <c r="I19" t="s">
-        <v>123</v>
-      </c>
-      <c r="J19" t="s">
-        <v>128</v>
-      </c>
       <c r="K19" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="L19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M19" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="O19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="1">
         <v>-250.3</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H20">
         <v>-58.2</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>0.23</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>28</v>
       </c>
-      <c r="I20" t="s">
-        <v>124</v>
-      </c>
-      <c r="J20" t="s">
-        <v>129</v>
-      </c>
       <c r="K20" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="L20" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M20" t="s">
+        <v>128</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21">
         <v>-242.6</v>
       </c>
       <c r="F21">
+        <v>15.67</v>
+      </c>
+      <c r="G21">
+        <v>188</v>
+      </c>
+      <c r="H21">
         <v>-59</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>0.13900000000000001</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>65</v>
       </c>
-      <c r="I21" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" t="s">
-        <v>128</v>
-      </c>
       <c r="K21" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="L21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M21" t="s">
+        <v>127</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="O21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22">
         <v>-247</v>
       </c>
       <c r="F22">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G22">
+        <v>414</v>
+      </c>
+      <c r="H22">
         <v>-49</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>0.24</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>28</v>
       </c>
-      <c r="I22" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" t="s">
-        <v>129</v>
-      </c>
       <c r="K22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" t="s">
+        <v>210</v>
+      </c>
+      <c r="M22" t="s">
+        <v>128</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O22" t="s">
         <v>51</v>
       </c>
-      <c r="L22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23">
         <v>-248.1</v>
       </c>
       <c r="F23">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G23">
+        <v>101</v>
+      </c>
+      <c r="H23">
         <v>-56</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>0.27</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>130</v>
       </c>
-      <c r="I23" t="s">
-        <v>123</v>
-      </c>
-      <c r="J23" t="s">
-        <v>129</v>
-      </c>
       <c r="K23" t="s">
+        <v>122</v>
+      </c>
+      <c r="L23" t="s">
+        <v>210</v>
+      </c>
+      <c r="M23" t="s">
+        <v>128</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O23" t="s">
         <v>55</v>
       </c>
-      <c r="L23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E24">
         <v>-239</v>
       </c>
       <c r="F24">
+        <v>21.7</v>
+      </c>
+      <c r="G24">
+        <v>240</v>
+      </c>
+      <c r="H24">
         <v>-50</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>0.17</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>22</v>
       </c>
-      <c r="I24" t="s">
-        <v>123</v>
-      </c>
-      <c r="J24" t="s">
-        <v>129</v>
-      </c>
       <c r="K24" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="L24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M24" t="s">
+        <v>128</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>0</v>
       </c>
       <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" t="s">
         <v>168</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D25" t="s">
-        <v>170</v>
       </c>
       <c r="E25">
         <v>-250.6</v>
       </c>
       <c r="F25">
+        <v>19.8</v>
+      </c>
+      <c r="G25">
+        <v>66.2</v>
+      </c>
+      <c r="H25">
         <v>-61</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>0.17</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>28</v>
       </c>
-      <c r="I25" t="s">
-        <v>124</v>
-      </c>
-      <c r="J25" t="s">
-        <v>129</v>
-      </c>
       <c r="K25" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="L25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M25" t="s">
+        <v>128</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="O25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" t="s">
         <v>173</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D26" t="s">
-        <v>175</v>
       </c>
       <c r="E26">
         <v>-243.2</v>
       </c>
       <c r="F26">
+        <v>2.5</v>
+      </c>
+      <c r="G26">
+        <v>397</v>
+      </c>
+      <c r="H26">
         <v>-54.8</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>2.75E-2</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>65</v>
       </c>
-      <c r="I26" t="s">
-        <v>126</v>
-      </c>
-      <c r="J26" t="s">
-        <v>128</v>
-      </c>
       <c r="K26" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="L26" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M26" t="s">
+        <v>127</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" t="s">
         <v>178</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D27" t="s">
-        <v>180</v>
       </c>
       <c r="E27">
         <v>-239.2</v>
       </c>
       <c r="F27">
+        <v>1.6</v>
+      </c>
+      <c r="G27">
+        <v>860</v>
+      </c>
+      <c r="H27">
         <v>-57</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>0.33</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>28</v>
       </c>
-      <c r="I27" t="s">
-        <v>123</v>
-      </c>
-      <c r="J27" t="s">
-        <v>129</v>
-      </c>
       <c r="K27" t="s">
-        <v>181</v>
+        <v>122</v>
       </c>
       <c r="L27" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="M27" t="s">
+        <v>128</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="O27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="b">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" t="s">
         <v>183</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D28" t="s">
-        <v>185</v>
       </c>
       <c r="E28">
         <v>-237</v>
       </c>
       <c r="F28">
+        <v>10.7</v>
+      </c>
+      <c r="G28">
+        <v>420</v>
+      </c>
+      <c r="H28">
         <v>-42</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>0.5</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>40</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K28" t="s">
-        <v>186</v>
-      </c>
-      <c r="L28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="b">
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29">
         <v>-230</v>
       </c>
       <c r="F29">
+        <v>20.9</v>
+      </c>
+      <c r="G29">
+        <v>557</v>
+      </c>
+      <c r="H29">
         <v>-73.7</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>0.77</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>65</v>
       </c>
-      <c r="I29" t="s">
-        <v>123</v>
-      </c>
-      <c r="J29" t="s">
-        <v>129</v>
-      </c>
       <c r="K29" t="s">
+        <v>122</v>
+      </c>
+      <c r="L29" t="s">
+        <v>210</v>
+      </c>
+      <c r="M29" t="s">
+        <v>128</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O29" t="s">
         <v>59</v>
       </c>
-      <c r="L29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="b">
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="D30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30">
         <v>-238.3</v>
       </c>
       <c r="F30">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G30">
+        <v>390</v>
+      </c>
+      <c r="H30">
         <v>-41</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>0.38</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>65</v>
       </c>
-      <c r="I30" t="s">
-        <v>123</v>
-      </c>
-      <c r="J30" t="s">
-        <v>129</v>
-      </c>
       <c r="K30" t="s">
+        <v>122</v>
+      </c>
+      <c r="L30" t="s">
+        <v>210</v>
+      </c>
+      <c r="M30" t="s">
+        <v>128</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O30" t="s">
         <v>63</v>
       </c>
-      <c r="L30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="b">
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31">
         <v>-249.8</v>
       </c>
       <c r="F31">
+        <v>16.7</v>
+      </c>
+      <c r="G31">
+        <v>79.3</v>
+      </c>
+      <c r="H31">
         <v>-63.6</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <v>0.22</v>
       </c>
-      <c r="H31">
+      <c r="J31">
         <v>28</v>
       </c>
-      <c r="I31" t="s">
-        <v>124</v>
-      </c>
-      <c r="J31" t="s">
-        <v>129</v>
-      </c>
       <c r="K31" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" t="s">
+        <v>213</v>
+      </c>
+      <c r="M31" t="s">
+        <v>128</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O31" t="s">
         <v>67</v>
       </c>
-      <c r="L31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="b">
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32">
         <v>-250.5</v>
       </c>
       <c r="F32">
+        <v>15.3</v>
+      </c>
+      <c r="G32">
+        <v>76</v>
+      </c>
+      <c r="H32">
         <v>-65</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <v>0.17</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>40</v>
       </c>
-      <c r="I32" t="s">
-        <v>124</v>
-      </c>
-      <c r="J32" t="s">
-        <v>129</v>
-      </c>
       <c r="K32" t="s">
+        <v>122</v>
+      </c>
+      <c r="L32" t="s">
+        <v>215</v>
+      </c>
+      <c r="M32" t="s">
+        <v>128</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O32" t="s">
         <v>71</v>
       </c>
-      <c r="L32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="b">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33">
         <v>-248</v>
       </c>
       <c r="F33">
+        <v>21</v>
+      </c>
+      <c r="G33">
+        <v>87.1</v>
+      </c>
+      <c r="H33">
         <v>-53.7</v>
       </c>
-      <c r="G33">
+      <c r="I33">
         <v>0.34</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>28</v>
       </c>
-      <c r="I33" t="s">
-        <v>124</v>
-      </c>
-      <c r="J33" t="s">
-        <v>129</v>
-      </c>
       <c r="K33" t="s">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="L33" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M33" t="s">
+        <v>128</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="b">
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E34">
         <v>-250.6</v>
       </c>
       <c r="F34">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G34">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="H34">
         <v>-60.3</v>
       </c>
-      <c r="G34">
+      <c r="I34">
         <v>0.36</v>
       </c>
-      <c r="H34">
+      <c r="J34">
         <v>28</v>
       </c>
-      <c r="I34" t="s">
-        <v>124</v>
-      </c>
-      <c r="J34" t="s">
-        <v>129</v>
-      </c>
       <c r="K34" t="s">
+        <v>122</v>
+      </c>
+      <c r="L34" t="s">
+        <v>213</v>
+      </c>
+      <c r="M34" t="s">
+        <v>128</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O34" t="s">
         <v>85</v>
       </c>
-      <c r="L34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="b">
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E35">
         <v>-242.6</v>
       </c>
       <c r="F35">
+        <v>15.67</v>
+      </c>
+      <c r="G35">
+        <v>188</v>
+      </c>
+      <c r="H35">
         <v>-60</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <v>0.13900000000000001</v>
       </c>
-      <c r="H35">
+      <c r="J35">
         <v>65</v>
       </c>
-      <c r="I35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J35" t="s">
-        <v>128</v>
-      </c>
       <c r="K35" t="s">
+        <v>122</v>
+      </c>
+      <c r="L35" t="s">
+        <v>210</v>
+      </c>
+      <c r="M35" t="s">
+        <v>127</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O35" t="s">
         <v>93</v>
       </c>
-      <c r="L35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="b">
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E36">
         <v>-251.7</v>
       </c>
       <c r="F36">
+        <v>10.8</v>
+      </c>
+      <c r="G36">
+        <v>107.6</v>
+      </c>
+      <c r="H36">
         <v>-50.4</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <v>0.21</v>
       </c>
-      <c r="H36">
+      <c r="J36">
         <v>28</v>
       </c>
-      <c r="I36" t="s">
-        <v>124</v>
-      </c>
-      <c r="J36" t="s">
-        <v>129</v>
-      </c>
       <c r="K36" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
       <c r="L36" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="M36" t="s">
+        <v>128</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="b">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>101</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>205</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E37">
-        <v>-251</v>
+        <v>-233.8</v>
       </c>
       <c r="F37">
-        <v>-61</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="G37">
-        <v>0.21</v>
+        <v>648</v>
       </c>
       <c r="H37">
+        <v>-58</v>
+      </c>
+      <c r="I37">
+        <v>0.108</v>
+      </c>
+      <c r="J37">
         <v>65</v>
       </c>
-      <c r="I37" t="s">
-        <v>124</v>
-      </c>
-      <c r="J37" t="s">
-        <v>129</v>
-      </c>
       <c r="K37" t="s">
-        <v>206</v>
+        <v>122</v>
       </c>
       <c r="L37" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M37" t="s">
+        <v>127</v>
+      </c>
+      <c r="N37" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D38" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38">
-        <v>-233.8</v>
-      </c>
-      <c r="F38">
-        <v>-58</v>
-      </c>
-      <c r="G38">
-        <v>0.108</v>
-      </c>
-      <c r="H38">
-        <v>65</v>
-      </c>
-      <c r="I38" t="s">
-        <v>123</v>
-      </c>
-      <c r="J38" t="s">
-        <v>128</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="O37" t="s">
         <v>104</v>
       </c>
-      <c r="L38" t="s">
-        <v>105</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" xr:uid="{E232B5B4-E744-4E0B-B74E-3A04EF1AEFB3}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{0552F544-F0DF-4D55-8249-04CEAD860409}"/>
+    <hyperlink ref="N37" r:id="rId3" xr:uid="{55C109CE-5924-4938-84F7-DC204AAF8498}"/>
+    <hyperlink ref="N36" r:id="rId4" xr:uid="{3B969C18-0841-400E-8B75-7DAFC84A97CA}"/>
+    <hyperlink ref="N35" r:id="rId5" xr:uid="{B3D4B7F3-1A1F-4E62-B6FA-A10970EB983E}"/>
+    <hyperlink ref="N34" r:id="rId6" xr:uid="{18C51F5D-A33C-401D-AB3E-A63671D0A04A}"/>
+    <hyperlink ref="N33" r:id="rId7" xr:uid="{D7E1F942-4441-4747-A77E-732FDFD2599A}"/>
+    <hyperlink ref="N32" r:id="rId8" xr:uid="{028A896E-079E-49D9-836C-8D977A498D2D}"/>
+    <hyperlink ref="N31" r:id="rId9" xr:uid="{53C48B87-16DD-4255-B3D5-436CB6FC1B5A}"/>
+    <hyperlink ref="N30" r:id="rId10" xr:uid="{8DFB28FC-7A01-49A8-AC0B-170F9DEAAAB4}"/>
+    <hyperlink ref="N29" r:id="rId11" xr:uid="{26C50D4D-B39A-4BEE-8922-8A7309EF0292}"/>
+    <hyperlink ref="N28" r:id="rId12" xr:uid="{E69BF196-16B7-4364-903A-2123B43A87A3}"/>
+    <hyperlink ref="N27" r:id="rId13" xr:uid="{C41406A6-917F-4E8D-B390-4332AFB727AB}"/>
+    <hyperlink ref="N26" r:id="rId14" xr:uid="{4510B694-D5FC-4DB3-861B-F3793CF682D9}"/>
+    <hyperlink ref="N25" r:id="rId15" xr:uid="{C5C68201-E1F1-4EB5-9D92-075C7CE22A2E}"/>
+    <hyperlink ref="N24" r:id="rId16" xr:uid="{678EE13B-2A37-46E2-A947-E4B14D73BFBE}"/>
+    <hyperlink ref="N23" r:id="rId17" xr:uid="{A8FBD716-533C-4303-86BF-F3C388B7B070}"/>
+    <hyperlink ref="N22" r:id="rId18" xr:uid="{97DA02D1-A5F4-49B1-B4DC-ACBA8E50454A}"/>
+    <hyperlink ref="N21" r:id="rId19" xr:uid="{8DFEAF18-73B3-4E4A-924B-3BEBB5BBE098}"/>
+    <hyperlink ref="N20" r:id="rId20" xr:uid="{ED849692-445E-485A-8CFA-C96333C6829E}"/>
+    <hyperlink ref="N19" r:id="rId21" xr:uid="{0D9C2A66-F9CA-43AC-AB7D-D71CF2D8B664}"/>
+    <hyperlink ref="N18" r:id="rId22" xr:uid="{0CFBD616-FE63-45C3-A5CF-65E0685A27D2}"/>
+    <hyperlink ref="N17" r:id="rId23" xr:uid="{26D68220-1314-4C15-A8BD-E0882DF8DB5B}"/>
+    <hyperlink ref="N16" r:id="rId24" xr:uid="{992A3000-449E-4B9B-BA03-B2A2790EEECC}"/>
+    <hyperlink ref="N15" r:id="rId25" xr:uid="{22A3DEE5-CCD3-4CFC-BA6C-E0E5BC1CFBC5}"/>
+    <hyperlink ref="N14" r:id="rId26" xr:uid="{308D753C-BE30-444C-A951-A9F9A6C229B7}"/>
+    <hyperlink ref="N13" r:id="rId27" xr:uid="{714B659D-D4AF-46E2-91E7-5661F823920C}"/>
+    <hyperlink ref="N12" r:id="rId28" xr:uid="{7A34D073-296E-4228-B6F9-7D19F31A3C46}"/>
+    <hyperlink ref="N11" r:id="rId29" xr:uid="{5ABA6C2A-E0D9-43F1-8C30-427ABD013790}"/>
+    <hyperlink ref="N10" r:id="rId30" xr:uid="{56C8C4C6-94D9-4798-9BCC-875966148F14}"/>
+    <hyperlink ref="N9" r:id="rId31" xr:uid="{A3D85411-0B02-49B0-A94A-1431B7EA57E2}"/>
+    <hyperlink ref="N8" r:id="rId32" xr:uid="{6685A9BE-E8A9-46B7-8259-89DEE2AB0A56}"/>
+    <hyperlink ref="N7" r:id="rId33" xr:uid="{CC7442BF-8449-47F3-B83F-F07DC77C8B69}"/>
+    <hyperlink ref="N6" r:id="rId34" xr:uid="{585670AC-1996-48D5-8CEB-C132C62B805F}"/>
+    <hyperlink ref="N5" r:id="rId35" xr:uid="{646F44DE-6CBC-4EF5-B333-1D33428DAB24}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB5F0F7-BBC3-4CAC-89BB-3F77AF195CCD}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="140.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3258,311 +3665,395 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" t="s">
         <v>120</v>
       </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>121</v>
       </c>
-      <c r="H1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2">
         <v>-250</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>-71.900000000000006</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.33</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I2" t="s">
-        <v>129</v>
-      </c>
       <c r="J2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" t="s">
         <v>89</v>
       </c>
-      <c r="K2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3">
         <v>-249.1</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>-68</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.12</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" t="s">
-        <v>129</v>
-      </c>
       <c r="J3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
         <v>77</v>
       </c>
-      <c r="K3" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>-253.5</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>-63.4</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.21</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
-        <v>124</v>
-      </c>
-      <c r="I4" t="s">
-        <v>129</v>
-      </c>
       <c r="J4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" t="s">
         <v>81</v>
       </c>
-      <c r="K4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5">
         <v>-247.4</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>-62.1</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.23</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>65</v>
       </c>
-      <c r="H5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I5" t="s">
-        <v>129</v>
-      </c>
       <c r="J5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K5" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" t="s">
         <v>74</v>
       </c>
-      <c r="K5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="1">
         <v>-250.3</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6">
         <v>-58.2</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.23</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>28</v>
       </c>
-      <c r="H6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I6" t="s">
-        <v>129</v>
-      </c>
       <c r="J6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K6" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>194</v>
       </c>
-      <c r="K6" t="s">
+      <c r="B7" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7">
         <v>-249.4</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>-59</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.31</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>40</v>
       </c>
-      <c r="H7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" t="s">
-        <v>129</v>
-      </c>
       <c r="J7" t="s">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="K7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8">
         <v>-239.1</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>-63</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.14599999999999999</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>65</v>
       </c>
-      <c r="H8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I8" t="s">
-        <v>128</v>
-      </c>
       <c r="J8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K8" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" t="s">
         <v>97</v>
       </c>
-      <c r="L8" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>99</v>
-      </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9">
         <v>-250.3</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>-56</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>0.27</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>130</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
+        <v>122</v>
+      </c>
+      <c r="K9" t="s">
+        <v>128</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10">
+        <v>-251</v>
+      </c>
+      <c r="G10">
+        <v>-61</v>
+      </c>
+      <c r="H10">
+        <v>0.21</v>
+      </c>
+      <c r="I10">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
         <v>123</v>
       </c>
-      <c r="I9" t="s">
-        <v>129</v>
-      </c>
-      <c r="J9" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" t="s">
-        <v>101</v>
+      <c r="K10" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="M10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{266BE416-15E0-477B-B543-FB1FBA9FF118}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{B7524E60-BCF8-44A7-86A6-739FC6DBA017}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{2AC54F9D-20F4-49DD-9A0E-D50A8A452EE1}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{D1AEBA4D-A9EF-4FB7-95A6-063BB1B2C485}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{8CE20859-BF76-4706-8D23-720786769B7E}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{C77F9676-7255-4FCC-B0DD-2660C5F2F1BA}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{78F63B0A-9BD6-44A1-B1FE-FCF3AF7D1B06}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{2007C615-0D19-440B-8A2B-66D85E17C082}"/>
+    <hyperlink ref="L10" r:id="rId9" xr:uid="{B249629B-5794-4D17-B6AA-ACCB7EC3AC19}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E1BD0F-EFEB-4E4C-842D-B057DB7CF8BC}">
+  <dimension ref="B4:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="61" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BUG: typos in readme and cleanup on references
</commit_message>
<xml_diff>
--- a/pll_data.xlsx
+++ b/pll_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETH\PhD\PLL_survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8275D3EE-69D1-46E1-B89F-1D390FE884CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BED845-AC69-4B62-81DE-464E6DFBCF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC291710-661A-4111-9329-6CD384A593DB}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -949,6 +949,18 @@
   </si>
   <si>
     <t>Put your own results here for comparison</t>
+  </si>
+  <si>
+    <t>MDLL/DPLL</t>
+  </si>
+  <si>
+    <t>BB/BB</t>
+  </si>
+  <si>
+    <t>DPLL/DPLL</t>
+  </si>
+  <si>
+    <t>SS/BB</t>
   </si>
 </sst>
 </file>
@@ -1852,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB6C843-7974-497E-9814-12CC7D1E0204}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1979,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="E3">
         <v>-249.1</v>
@@ -2014,7 +2026,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>216</v>
       </c>
       <c r="E4">
         <v>-253.5</v>
@@ -2129,10 +2141,10 @@
         <v>65</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>122</v>
+        <v>219</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>128</v>
@@ -2411,10 +2423,10 @@
         <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>122</v>
+        <v>221</v>
       </c>
       <c r="L12" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="M12" t="s">
         <v>128</v>
@@ -3462,142 +3474,95 @@
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>198</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E35">
-        <v>-242.6</v>
+        <v>-251.7</v>
       </c>
       <c r="F35">
-        <v>15.67</v>
+        <v>10.8</v>
       </c>
       <c r="G35">
-        <v>188</v>
+        <v>107.6</v>
       </c>
       <c r="H35">
-        <v>-60</v>
+        <v>-50.4</v>
       </c>
       <c r="I35">
-        <v>0.13900000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="J35">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="K35" t="s">
         <v>122</v>
       </c>
       <c r="L35" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="O35" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>199</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E36">
-        <v>-251.7</v>
+        <v>-233.8</v>
       </c>
       <c r="F36">
-        <v>10.8</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="G36">
-        <v>107.6</v>
+        <v>648</v>
       </c>
       <c r="H36">
-        <v>-50.4</v>
+        <v>-58</v>
       </c>
       <c r="I36">
-        <v>0.21</v>
+        <v>0.108</v>
       </c>
       <c r="J36">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="K36" t="s">
         <v>122</v>
       </c>
       <c r="L36" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>200</v>
+        <v>103</v>
       </c>
       <c r="O36" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" t="s">
-        <v>116</v>
-      </c>
-      <c r="E37">
-        <v>-233.8</v>
-      </c>
-      <c r="F37">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="G37">
-        <v>648</v>
-      </c>
-      <c r="H37">
-        <v>-58</v>
-      </c>
-      <c r="I37">
-        <v>0.108</v>
-      </c>
-      <c r="J37">
-        <v>65</v>
-      </c>
-      <c r="K37" t="s">
-        <v>122</v>
-      </c>
-      <c r="L37" t="s">
-        <v>210</v>
-      </c>
-      <c r="M37" t="s">
-        <v>127</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O37" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3605,59 +3570,60 @@
   <hyperlinks>
     <hyperlink ref="N3" r:id="rId1" xr:uid="{E232B5B4-E744-4E0B-B74E-3A04EF1AEFB3}"/>
     <hyperlink ref="N4" r:id="rId2" xr:uid="{0552F544-F0DF-4D55-8249-04CEAD860409}"/>
-    <hyperlink ref="N37" r:id="rId3" xr:uid="{55C109CE-5924-4938-84F7-DC204AAF8498}"/>
-    <hyperlink ref="N36" r:id="rId4" xr:uid="{3B969C18-0841-400E-8B75-7DAFC84A97CA}"/>
-    <hyperlink ref="N35" r:id="rId5" xr:uid="{B3D4B7F3-1A1F-4E62-B6FA-A10970EB983E}"/>
-    <hyperlink ref="N34" r:id="rId6" xr:uid="{18C51F5D-A33C-401D-AB3E-A63671D0A04A}"/>
-    <hyperlink ref="N33" r:id="rId7" xr:uid="{D7E1F942-4441-4747-A77E-732FDFD2599A}"/>
-    <hyperlink ref="N32" r:id="rId8" xr:uid="{028A896E-079E-49D9-836C-8D977A498D2D}"/>
-    <hyperlink ref="N31" r:id="rId9" xr:uid="{53C48B87-16DD-4255-B3D5-436CB6FC1B5A}"/>
-    <hyperlink ref="N30" r:id="rId10" xr:uid="{8DFB28FC-7A01-49A8-AC0B-170F9DEAAAB4}"/>
-    <hyperlink ref="N29" r:id="rId11" xr:uid="{26C50D4D-B39A-4BEE-8922-8A7309EF0292}"/>
-    <hyperlink ref="N28" r:id="rId12" xr:uid="{E69BF196-16B7-4364-903A-2123B43A87A3}"/>
-    <hyperlink ref="N27" r:id="rId13" xr:uid="{C41406A6-917F-4E8D-B390-4332AFB727AB}"/>
-    <hyperlink ref="N26" r:id="rId14" xr:uid="{4510B694-D5FC-4DB3-861B-F3793CF682D9}"/>
-    <hyperlink ref="N25" r:id="rId15" xr:uid="{C5C68201-E1F1-4EB5-9D92-075C7CE22A2E}"/>
-    <hyperlink ref="N24" r:id="rId16" xr:uid="{678EE13B-2A37-46E2-A947-E4B14D73BFBE}"/>
-    <hyperlink ref="N23" r:id="rId17" xr:uid="{A8FBD716-533C-4303-86BF-F3C388B7B070}"/>
-    <hyperlink ref="N22" r:id="rId18" xr:uid="{97DA02D1-A5F4-49B1-B4DC-ACBA8E50454A}"/>
-    <hyperlink ref="N21" r:id="rId19" xr:uid="{8DFEAF18-73B3-4E4A-924B-3BEBB5BBE098}"/>
-    <hyperlink ref="N20" r:id="rId20" xr:uid="{ED849692-445E-485A-8CFA-C96333C6829E}"/>
-    <hyperlink ref="N19" r:id="rId21" xr:uid="{0D9C2A66-F9CA-43AC-AB7D-D71CF2D8B664}"/>
-    <hyperlink ref="N18" r:id="rId22" xr:uid="{0CFBD616-FE63-45C3-A5CF-65E0685A27D2}"/>
-    <hyperlink ref="N17" r:id="rId23" xr:uid="{26D68220-1314-4C15-A8BD-E0882DF8DB5B}"/>
-    <hyperlink ref="N16" r:id="rId24" xr:uid="{992A3000-449E-4B9B-BA03-B2A2790EEECC}"/>
-    <hyperlink ref="N15" r:id="rId25" xr:uid="{22A3DEE5-CCD3-4CFC-BA6C-E0E5BC1CFBC5}"/>
-    <hyperlink ref="N14" r:id="rId26" xr:uid="{308D753C-BE30-444C-A951-A9F9A6C229B7}"/>
-    <hyperlink ref="N13" r:id="rId27" xr:uid="{714B659D-D4AF-46E2-91E7-5661F823920C}"/>
-    <hyperlink ref="N12" r:id="rId28" xr:uid="{7A34D073-296E-4228-B6F9-7D19F31A3C46}"/>
-    <hyperlink ref="N11" r:id="rId29" xr:uid="{5ABA6C2A-E0D9-43F1-8C30-427ABD013790}"/>
-    <hyperlink ref="N10" r:id="rId30" xr:uid="{56C8C4C6-94D9-4798-9BCC-875966148F14}"/>
-    <hyperlink ref="N9" r:id="rId31" xr:uid="{A3D85411-0B02-49B0-A94A-1431B7EA57E2}"/>
-    <hyperlink ref="N8" r:id="rId32" xr:uid="{6685A9BE-E8A9-46B7-8259-89DEE2AB0A56}"/>
-    <hyperlink ref="N7" r:id="rId33" xr:uid="{CC7442BF-8449-47F3-B83F-F07DC77C8B69}"/>
-    <hyperlink ref="N6" r:id="rId34" xr:uid="{585670AC-1996-48D5-8CEB-C132C62B805F}"/>
-    <hyperlink ref="N5" r:id="rId35" xr:uid="{646F44DE-6CBC-4EF5-B333-1D33428DAB24}"/>
+    <hyperlink ref="N36" r:id="rId3" xr:uid="{55C109CE-5924-4938-84F7-DC204AAF8498}"/>
+    <hyperlink ref="N35" r:id="rId4" xr:uid="{3B969C18-0841-400E-8B75-7DAFC84A97CA}"/>
+    <hyperlink ref="N34" r:id="rId5" xr:uid="{18C51F5D-A33C-401D-AB3E-A63671D0A04A}"/>
+    <hyperlink ref="N33" r:id="rId6" xr:uid="{D7E1F942-4441-4747-A77E-732FDFD2599A}"/>
+    <hyperlink ref="N32" r:id="rId7" xr:uid="{028A896E-079E-49D9-836C-8D977A498D2D}"/>
+    <hyperlink ref="N31" r:id="rId8" xr:uid="{53C48B87-16DD-4255-B3D5-436CB6FC1B5A}"/>
+    <hyperlink ref="N30" r:id="rId9" xr:uid="{8DFB28FC-7A01-49A8-AC0B-170F9DEAAAB4}"/>
+    <hyperlink ref="N29" r:id="rId10" xr:uid="{26C50D4D-B39A-4BEE-8922-8A7309EF0292}"/>
+    <hyperlink ref="N28" r:id="rId11" xr:uid="{E69BF196-16B7-4364-903A-2123B43A87A3}"/>
+    <hyperlink ref="N27" r:id="rId12" xr:uid="{C41406A6-917F-4E8D-B390-4332AFB727AB}"/>
+    <hyperlink ref="N26" r:id="rId13" xr:uid="{4510B694-D5FC-4DB3-861B-F3793CF682D9}"/>
+    <hyperlink ref="N25" r:id="rId14" xr:uid="{C5C68201-E1F1-4EB5-9D92-075C7CE22A2E}"/>
+    <hyperlink ref="N24" r:id="rId15" xr:uid="{678EE13B-2A37-46E2-A947-E4B14D73BFBE}"/>
+    <hyperlink ref="N23" r:id="rId16" xr:uid="{A8FBD716-533C-4303-86BF-F3C388B7B070}"/>
+    <hyperlink ref="N22" r:id="rId17" xr:uid="{97DA02D1-A5F4-49B1-B4DC-ACBA8E50454A}"/>
+    <hyperlink ref="N21" r:id="rId18" xr:uid="{8DFEAF18-73B3-4E4A-924B-3BEBB5BBE098}"/>
+    <hyperlink ref="N20" r:id="rId19" xr:uid="{ED849692-445E-485A-8CFA-C96333C6829E}"/>
+    <hyperlink ref="N19" r:id="rId20" xr:uid="{0D9C2A66-F9CA-43AC-AB7D-D71CF2D8B664}"/>
+    <hyperlink ref="N18" r:id="rId21" xr:uid="{0CFBD616-FE63-45C3-A5CF-65E0685A27D2}"/>
+    <hyperlink ref="N17" r:id="rId22" xr:uid="{26D68220-1314-4C15-A8BD-E0882DF8DB5B}"/>
+    <hyperlink ref="N16" r:id="rId23" xr:uid="{992A3000-449E-4B9B-BA03-B2A2790EEECC}"/>
+    <hyperlink ref="N15" r:id="rId24" xr:uid="{22A3DEE5-CCD3-4CFC-BA6C-E0E5BC1CFBC5}"/>
+    <hyperlink ref="N14" r:id="rId25" xr:uid="{308D753C-BE30-444C-A951-A9F9A6C229B7}"/>
+    <hyperlink ref="N13" r:id="rId26" xr:uid="{714B659D-D4AF-46E2-91E7-5661F823920C}"/>
+    <hyperlink ref="N12" r:id="rId27" xr:uid="{7A34D073-296E-4228-B6F9-7D19F31A3C46}"/>
+    <hyperlink ref="N11" r:id="rId28" xr:uid="{5ABA6C2A-E0D9-43F1-8C30-427ABD013790}"/>
+    <hyperlink ref="N10" r:id="rId29" xr:uid="{56C8C4C6-94D9-4798-9BCC-875966148F14}"/>
+    <hyperlink ref="N9" r:id="rId30" xr:uid="{A3D85411-0B02-49B0-A94A-1431B7EA57E2}"/>
+    <hyperlink ref="N8" r:id="rId31" xr:uid="{6685A9BE-E8A9-46B7-8259-89DEE2AB0A56}"/>
+    <hyperlink ref="N7" r:id="rId32" xr:uid="{CC7442BF-8449-47F3-B83F-F07DC77C8B69}"/>
+    <hyperlink ref="N6" r:id="rId33" xr:uid="{585670AC-1996-48D5-8CEB-C132C62B805F}"/>
+    <hyperlink ref="N5" r:id="rId34" xr:uid="{646F44DE-6CBC-4EF5-B333-1D33428DAB24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB5F0F7-BBC3-4CAC-89BB-3F77AF195CCD}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="140.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="140.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3689,16 +3655,19 @@
         <v>121</v>
       </c>
       <c r="K1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L1" t="s">
         <v>126</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -3723,17 +3692,17 @@
       <c r="J2" t="s">
         <v>123</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>128</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -3758,17 +3727,17 @@
       <c r="J3" t="s">
         <v>124</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>128</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -3793,17 +3762,17 @@
       <c r="J4" t="s">
         <v>123</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>128</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -3828,17 +3797,17 @@
       <c r="J5" t="s">
         <v>123</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>128</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -3865,17 +3834,17 @@
       <c r="J6" t="s">
         <v>123</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>128</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -3900,17 +3869,17 @@
       <c r="J7" t="s">
         <v>122</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>128</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -3935,17 +3904,17 @@
       <c r="J8" t="s">
         <v>122</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>127</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -3970,17 +3939,17 @@
       <c r="J9" t="s">
         <v>122</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>128</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>202</v>
       </c>
@@ -4005,27 +3974,72 @@
       <c r="J10" t="s">
         <v>123</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>128</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11">
+        <v>-242.6</v>
+      </c>
+      <c r="E11">
+        <v>15.67</v>
+      </c>
+      <c r="F11">
+        <v>188</v>
+      </c>
+      <c r="G11">
+        <v>-60</v>
+      </c>
+      <c r="H11">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="I11">
+        <v>65</v>
+      </c>
+      <c r="J11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" t="s">
+        <v>210</v>
+      </c>
+      <c r="L11" t="s">
+        <v>127</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{266BE416-15E0-477B-B543-FB1FBA9FF118}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{B7524E60-BCF8-44A7-86A6-739FC6DBA017}"/>
-    <hyperlink ref="L4" r:id="rId3" xr:uid="{2AC54F9D-20F4-49DD-9A0E-D50A8A452EE1}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{D1AEBA4D-A9EF-4FB7-95A6-063BB1B2C485}"/>
-    <hyperlink ref="L6" r:id="rId5" xr:uid="{8CE20859-BF76-4706-8D23-720786769B7E}"/>
-    <hyperlink ref="L7" r:id="rId6" xr:uid="{C77F9676-7255-4FCC-B0DD-2660C5F2F1BA}"/>
-    <hyperlink ref="L8" r:id="rId7" xr:uid="{78F63B0A-9BD6-44A1-B1FE-FCF3AF7D1B06}"/>
-    <hyperlink ref="L9" r:id="rId8" xr:uid="{2007C615-0D19-440B-8A2B-66D85E17C082}"/>
-    <hyperlink ref="L10" r:id="rId9" xr:uid="{B249629B-5794-4D17-B6AA-ACCB7EC3AC19}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{266BE416-15E0-477B-B543-FB1FBA9FF118}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{B7524E60-BCF8-44A7-86A6-739FC6DBA017}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{2AC54F9D-20F4-49DD-9A0E-D50A8A452EE1}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{D1AEBA4D-A9EF-4FB7-95A6-063BB1B2C485}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{8CE20859-BF76-4706-8D23-720786769B7E}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{C77F9676-7255-4FCC-B0DD-2660C5F2F1BA}"/>
+    <hyperlink ref="M8" r:id="rId7" xr:uid="{78F63B0A-9BD6-44A1-B1FE-FCF3AF7D1B06}"/>
+    <hyperlink ref="M9" r:id="rId8" xr:uid="{2007C615-0D19-440B-8A2B-66D85E17C082}"/>
+    <hyperlink ref="M10" r:id="rId9" xr:uid="{B249629B-5794-4D17-B6AA-ACCB7EC3AC19}"/>
+    <hyperlink ref="M11" r:id="rId10" xr:uid="{B3D4B7F3-1A1F-4E62-B6FA-A10970EB983E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ENH: additional references from JSCC Oct.2024 to Mar. 2025
</commit_message>
<xml_diff>
--- a/pll_data.xlsx
+++ b/pll_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETH\PhD\PLL_survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BED845-AC69-4B62-81DE-464E6DFBCF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6E4A67-5EFB-4530-A30B-B989A7EE4EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC291710-661A-4111-9329-6CD384A593DB}"/>
+    <workbookView xWindow="5580" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{CC291710-661A-4111-9329-6CD384A593DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="268">
   <si>
     <t>Name</t>
   </si>
@@ -961,6 +961,189 @@
   </si>
   <si>
     <t>SS/BB</t>
+  </si>
+  <si>
+    <t>JSSC'25</t>
+  </si>
+  <si>
+    <t>A Compact 20–24-GHz Sub-Sampling PLL With Charge-Domain Bandwidth Control Scheme</t>
+  </si>
+  <si>
+    <t>Wang, Li
+Liu, Zilu
+Ma, Ruitao
+Yue, C. Patrick</t>
+  </si>
+  <si>
+    <t>APLL</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10746381</t>
+  </si>
+  <si>
+    <t>Bandwidth, Capacitors, Compact, Frequency control, Gain, Gain control, Low-pass filters, Noise, Phase locked loops, Voltage-controlled oscillators, dual path (DP), integer-N, integral, jitter, phase-locked loop (PLL), proportional, sub-sampling, true single-phase clock (TSPC)</t>
+  </si>
+  <si>
+    <t>An Ultra-Low-Jitter Fast-Hopping Fractional-N PLL With LC DTC and Hybrid-Proportional Paths</t>
+  </si>
+  <si>
+    <t>Liu, Hongzhuo
+Deng, Wei
+Jia, Haikun
+Wang, Zhihua
+Chi, Baoyong</t>
+  </si>
+  <si>
+    <t>APLL/DPLL</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10843985</t>
+  </si>
+  <si>
+    <t>Bandwidth, Clocks, Counter, Delays, Frequency modulation, Phase frequency detectors, Phase locked loops, Tuning, Voltage-controlled oscillators, fast lock, frequency hopping, jitter, phase noise, sampling phase detector (SPD)</t>
+  </si>
+  <si>
+    <t>A Low-Jitter and Low-Reference-Spur Ring-VCO-Based Injection-Locked Clock Multiplier Utilizing a Complementary-Injection Scheme and an Adaptive Pulsewidth Adjustment</t>
+  </si>
+  <si>
+    <t>Wang, Zedong
+Zheng, Xuqiang
+He, Yu
+Xu, Hua
+Li, Sai
+Yang, Zunsong
+Lv, Fangxu
+Lai, Mingche
+Liu, Xinyu</t>
+  </si>
+  <si>
+    <t>ILCM</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10742924</t>
+  </si>
+  <si>
+    <t>Adaptive pulse generator (APG), Bandwidth, Clocks, Computer architecture, Delays, Noise reduction, Oscillators, Phase locked loops, Pulse generation, Voltage-controlled oscillators, complementary injection, frequency tracking loop (FTL), injection-locked clock multiplier (ILCM), jitter, noise suppression, optimal injection pulsewidth, phase error cancellation, ring voltage-controlled oscillator (RVCO)</t>
+  </si>
+  <si>
+    <t>A 12.24-GHz MDLL With a 102-Multiplication Factor Using a Power-Gating-Based Ring Oscillator</t>
+  </si>
+  <si>
+    <t>Cho, Yoonseo
+Lee, Jeonghyun
+Park, Suneui
+Yoo, Seyeon
+Choi, Jaehyouk</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10620066</t>
+  </si>
+  <si>
+    <t>Calibration, Clocks, Delays, Generators, Phase locked loops, Switches, jitter, multiplication factor (N), multiplying delay-locked loop (MDLL), power gating (PG), ring oscillator (RO)</t>
+  </si>
+  <si>
+    <t>A Transformer-Based Series-Resonance CMOS VCO</t>
+  </si>
+  <si>
+    <t>Zhang, Shiwei
+Deng, Wei
+Jia, Haikun
+Liu, Hongzhuo
+Sun, Shiyan
+Guan, Pingda
+Wang, Zhihua
+Chi, Baoyong</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10623620</t>
+  </si>
+  <si>
+    <t>CMOS, MOS devices, Oscillators, Phase locked loops, Resistance, Transformers, Voltage-controlled oscillators, jitter, millimeter-wave (mm-wave), oscillator, phase noise (PN), resonator, voltage-controlled oscillator (VCO)</t>
+  </si>
+  <si>
+    <t>An Ultra-Low-Voltage Bias-Current-Free Fractional-N Hybrid PLL With Voltage-Mode Phase Detection and Interpolation</t>
+  </si>
+  <si>
+    <t>Feng, Liqun
+Ji, Xuansheng
+Kuang, Longhao
+Liao, Qianxian
+Han, Su
+Zhao, Jiahao
+Rhee, Woogeun
+Wang, Zhihua</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10684576</t>
+  </si>
+  <si>
+    <t>Bias-current-free, Fractional-N, Interpolation, Linearity, Low voltage, Noise, Phase locked loops, Voltage-controlled oscillators, flip-flop phase detector (FFPD), hybrid, passive intensive, phase interpolator (PI), phase-locked loop (PLL), pseudo-differential, quantization noise (Q-noise), reference spur, time interleaved, ultra-low voltage (ULV), voltage, voltage mode</t>
+  </si>
+  <si>
+    <t>A 10-GHz Digital-PLL-Based Chirp Generator With Parabolic Non-Uniform Digital Predistortion for FMCW Radars</t>
+  </si>
+  <si>
+    <t>Tesolin, Francesco
+Dartizio, Simone M.
+Castoro, Giacomo
+Buccoleri, Francesco
+Rossoni, Michele
+Samori, Carlo
+Lacaita, Andrea L.
+Levantino, Salvatore</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10693572</t>
+  </si>
+  <si>
+    <t>Background calibration, Capacitors, Chirp, Digital phase-locked loop (DPLL), Frequency modulation, Generators, Radar, Tuning, digital pre-distortion (DPD), digitally controlled oscillator (DCO), fractional-N DPLL, frequency-modulated continuous-wave (FMCW) radar, multi-gain least-mean-square (LMS) algorithm, parabolic uniform DPD, phase noise, sawtooth chirp, two-point modulation (TPM)</t>
+  </si>
+  <si>
+    <t>A 7.5-GHz Subharmonic Injection-Locked Clock Multiplier Featuring a 120× Multiplying Factor and 92.3-fs RMS Jitter Including Reference Spur</t>
+  </si>
+  <si>
+    <t>Choi, Hangil
+Cho, SeongHwan</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10702551</t>
+  </si>
+  <si>
+    <t>Calibration, Clocks, Frequency synthesizer, Phase distortion, Phase locked loops, Switches, Time-frequency analysis, Timing, Voltage-controlled oscillators, jitter, low-jitter, low-reference spur, phase noise, phase-locked loop (PLL), subharmonic injection-locked clock multiplier (SILCM), voltage-controlled oscillator (VCO)</t>
+  </si>
+  <si>
+    <t>A 23.2-to-26-GHz Low-Jitter Fast-Locking Sub-Sampling PLL Based on a Function-Reused VCO-Buffer and a Type-I FLL With Rapid Phase Alignment</t>
+  </si>
+  <si>
+    <t>Li, Haoran
+Xu, Tailong
+Meng, Xi
+Yin, Jun
+Martins, Rui P.
+Mak, Pui-In</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10684529</t>
+  </si>
+  <si>
+    <t>Capacitance, Fast locking, Frequency conversion, Frequency locked loops, Frequency synthesizers, Phase locked loops, Voltage-controlled oscillators, frequency synthesis, frequency-locked loop (FLL), jitter, low jitter, millimeter-wave (mm-wave), phase-locked loop (PLL), reference (ref.) spur, sub-sampling phase detector (SSPD), voltage-controlled oscillator (VCO)</t>
+  </si>
+  <si>
+    <t>A Jitter Programmable Digital Bang-Bang PLL Using PVT-Invariant Stochastic Jitter Monitor</t>
+  </si>
+  <si>
+    <t>Kim, Yong-Jo
+Jang, Taekwang
+Cho, SeongHwan</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10536156</t>
+  </si>
+  <si>
+    <t>Bandwidth, Capacitors, Digital bang-bang phase-locked loop (DBPLL), Monitoring, Phase locked loops, System-on-chip, Voltage-controlled oscillators, jitter, process, ring oscillator, stochastic jitter monitoring circuit, voltage and temperature (PVT) variations</t>
   </si>
 </sst>
 </file>
@@ -1864,13 +2047,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB6C843-7974-497E-9814-12CC7D1E0204}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -1883,7 +2066,7 @@
     <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -1930,7 +2113,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1973,46 +2156,46 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>216</v>
       </c>
       <c r="E3">
-        <v>-249.1</v>
+        <v>-253.5</v>
       </c>
       <c r="F3">
-        <v>15.7</v>
+        <v>17.5</v>
       </c>
       <c r="G3">
-        <v>88</v>
+        <v>57.3</v>
       </c>
       <c r="H3">
-        <v>-68</v>
+        <v>-63.4</v>
       </c>
       <c r="I3">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
       <c r="J3">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>122</v>
       </c>
       <c r="L3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M3" t="s">
         <v>128</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2020,31 +2203,31 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>216</v>
       </c>
       <c r="E4">
-        <v>-253.5</v>
+        <v>-247.4</v>
       </c>
       <c r="F4">
-        <v>17.5</v>
+        <v>8.89</v>
       </c>
       <c r="G4">
-        <v>57.3</v>
+        <v>143.69999999999999</v>
       </c>
       <c r="H4">
-        <v>-63.4</v>
+        <v>-62.1</v>
       </c>
       <c r="I4">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="J4">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
         <v>122</v>
@@ -2056,10 +2239,10 @@
         <v>128</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2067,34 +2250,31 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>224</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>223</v>
       </c>
       <c r="E5">
-        <v>-251</v>
+        <v>-253</v>
       </c>
       <c r="F5">
-        <v>7.3</v>
+        <v>13.35</v>
       </c>
       <c r="G5">
-        <v>104</v>
-      </c>
-      <c r="H5">
-        <v>-58</v>
+        <v>61.23</v>
       </c>
       <c r="I5">
-        <v>0.21</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="J5">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>122</v>
+        <v>226</v>
       </c>
       <c r="L5" t="s">
         <v>215</v>
@@ -2103,10 +2283,10 @@
         <v>128</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>14</v>
+        <v>227</v>
       </c>
       <c r="O5" t="s">
-        <v>15</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2114,46 +2294,46 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>229</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E6">
-        <v>-242.9</v>
+        <v>-250.7</v>
       </c>
       <c r="F6">
-        <v>14.2</v>
-      </c>
-      <c r="G6">
-        <v>191</v>
-      </c>
-      <c r="H6" s="1">
-        <v>-52.7</v>
+        <v>34</v>
+      </c>
+      <c r="G6" s="1">
+        <v>41.3</v>
+      </c>
+      <c r="H6">
+        <v>-62.4</v>
       </c>
       <c r="I6">
-        <v>0.48</v>
-      </c>
-      <c r="J6" s="1">
-        <v>65</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="M6" s="1" t="s">
+        <v>0.21</v>
+      </c>
+      <c r="J6">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
+        <v>231</v>
+      </c>
+      <c r="L6" t="s">
+        <v>222</v>
+      </c>
+      <c r="M6" t="s">
         <v>128</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>18</v>
+        <v>232</v>
       </c>
       <c r="O6" t="s">
-        <v>19</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2161,46 +2341,43 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>234</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E7">
-        <v>-247.4</v>
+        <v>-255.5</v>
       </c>
       <c r="F7">
-        <v>8.89</v>
+        <v>14.5</v>
       </c>
       <c r="G7">
-        <v>143.69999999999999</v>
-      </c>
-      <c r="H7">
-        <v>-62.1</v>
+        <v>43.9</v>
       </c>
       <c r="I7">
-        <v>0.23</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="J7">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="K7" t="s">
-        <v>122</v>
+        <v>236</v>
       </c>
       <c r="L7" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="M7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>22</v>
+        <v>238</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2208,46 +2385,43 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>223</v>
       </c>
       <c r="E8">
-        <v>-246.2</v>
+        <v>-246.6</v>
       </c>
       <c r="F8">
-        <v>4.4000000000000004</v>
+        <v>14.7</v>
       </c>
       <c r="G8">
-        <v>233</v>
-      </c>
-      <c r="H8">
-        <v>-60.6</v>
+        <v>122</v>
       </c>
       <c r="I8">
-        <v>0.31</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="J8">
         <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L8" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>26</v>
+        <v>242</v>
       </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,46 +2429,43 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>131</v>
+        <v>245</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>223</v>
       </c>
       <c r="E9">
-        <v>-230.6</v>
+        <v>-245.6</v>
       </c>
       <c r="F9">
-        <v>13.56</v>
+        <v>242</v>
       </c>
       <c r="G9">
-        <v>1000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>-67</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="J9" s="1">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="I9">
+        <v>0.7</v>
+      </c>
+      <c r="J9">
         <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="L9" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="M9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="O9" t="s">
-        <v>133</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2302,28 +2473,28 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>248</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>249</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>223</v>
       </c>
       <c r="E10">
-        <v>-250</v>
+        <v>-245.5</v>
       </c>
       <c r="F10">
-        <v>17.2</v>
+        <v>0.78</v>
       </c>
       <c r="G10">
-        <v>77</v>
+        <v>610</v>
       </c>
       <c r="H10">
-        <v>-71.900000000000006</v>
+        <v>-57.2</v>
       </c>
       <c r="I10">
-        <v>0.33</v>
+        <v>0.24</v>
       </c>
       <c r="J10">
         <v>28</v>
@@ -2338,10 +2509,10 @@
         <v>128</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>30</v>
+        <v>250</v>
       </c>
       <c r="O10" t="s">
-        <v>31</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2349,46 +2520,46 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>223</v>
       </c>
       <c r="E11">
-        <v>-251.7</v>
+        <v>-242.9</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>14.2</v>
       </c>
       <c r="G11">
-        <v>59.78</v>
+        <v>191</v>
       </c>
       <c r="H11" s="1">
-        <v>-58.7</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.23</v>
+        <v>-52.7</v>
+      </c>
+      <c r="I11">
+        <v>0.48</v>
       </c>
       <c r="J11" s="1">
-        <v>28</v>
-      </c>
-      <c r="K11" t="s">
-        <v>122</v>
-      </c>
-      <c r="L11" t="s">
-        <v>213</v>
-      </c>
-      <c r="M11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>128</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="O11" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2396,46 +2567,46 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>139</v>
+        <v>253</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12">
-        <v>-250.6</v>
+        <v>-248</v>
       </c>
       <c r="F12">
-        <v>17.899999999999999</v>
+        <v>21</v>
       </c>
       <c r="G12">
-        <v>135</v>
+        <v>87.1</v>
       </c>
       <c r="H12">
-        <v>-57</v>
+        <v>-53.7</v>
       </c>
       <c r="I12">
-        <v>0.38</v>
+        <v>0.34</v>
       </c>
       <c r="J12">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="K12" t="s">
-        <v>221</v>
+        <v>122</v>
       </c>
       <c r="L12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="M12" t="s">
         <v>128</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="O12" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2443,93 +2614,87 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>256</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13">
-        <v>-249.4</v>
+        <v>-259.7</v>
       </c>
       <c r="F13">
-        <v>3.5</v>
-      </c>
-      <c r="G13">
-        <v>182</v>
-      </c>
-      <c r="H13" s="1">
-        <v>-59</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0.31</v>
-      </c>
-      <c r="J13" s="1">
-        <v>40</v>
+        <v>2.33</v>
+      </c>
+      <c r="G13" s="1">
+        <v>67.7</v>
+      </c>
+      <c r="I13">
+        <v>0.26</v>
+      </c>
+      <c r="J13">
+        <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>122</v>
+        <v>236</v>
       </c>
       <c r="L13" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="M13" t="s">
         <v>128</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>144</v>
+        <v>258</v>
       </c>
       <c r="O13" t="s">
-        <v>145</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>260</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>147</v>
+        <v>261</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14">
-        <v>-248.7</v>
+        <v>105</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-253.5</v>
       </c>
       <c r="F14">
-        <v>36</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G14">
-        <v>72</v>
-      </c>
-      <c r="H14">
-        <v>-59.7</v>
+        <v>48.3</v>
       </c>
       <c r="I14">
-        <v>0.47</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="J14">
         <v>28</v>
       </c>
       <c r="K14" t="s">
-        <v>122</v>
+        <v>226</v>
       </c>
       <c r="L14" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="M14" t="s">
         <v>128</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>148</v>
+        <v>262</v>
       </c>
       <c r="O14" t="s">
-        <v>149</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2537,28 +2702,25 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>264</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>265</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="1">
-        <v>-251.5</v>
-      </c>
-      <c r="F15" s="1">
-        <v>10.8</v>
-      </c>
-      <c r="G15" s="1">
-        <v>79.7</v>
-      </c>
-      <c r="H15">
-        <v>-51.1</v>
+        <v>105</v>
+      </c>
+      <c r="E15">
+        <v>-225</v>
+      </c>
+      <c r="F15">
+        <v>11.2</v>
+      </c>
+      <c r="G15">
+        <v>1680</v>
       </c>
       <c r="I15">
-        <v>0.21</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J15">
         <v>28</v>
@@ -2570,13 +2732,13 @@
         <v>213</v>
       </c>
       <c r="M15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>34</v>
+        <v>266</v>
       </c>
       <c r="O15" t="s">
-        <v>35</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2584,46 +2746,46 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E16">
-        <v>-224.8</v>
+        <v>-249.1</v>
       </c>
       <c r="F16">
-        <v>11.95</v>
+        <v>15.7</v>
       </c>
       <c r="G16">
-        <v>1670</v>
+        <v>88</v>
       </c>
       <c r="H16">
-        <v>-52</v>
+        <v>-68</v>
       </c>
       <c r="I16">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="J16">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="O16" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2631,46 +2793,46 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17">
-        <v>-242.3</v>
+        <v>-251</v>
       </c>
       <c r="F17">
-        <v>3.25</v>
+        <v>7.3</v>
       </c>
       <c r="G17">
-        <v>428</v>
-      </c>
-      <c r="H17" s="1">
-        <v>-55</v>
+        <v>104</v>
+      </c>
+      <c r="H17">
+        <v>-58</v>
       </c>
       <c r="I17">
-        <v>0.39</v>
-      </c>
-      <c r="J17" s="1">
-        <v>40</v>
-      </c>
-      <c r="K17" s="1" t="s">
+        <v>0.21</v>
+      </c>
+      <c r="J17">
+        <v>65</v>
+      </c>
+      <c r="K17" t="s">
         <v>122</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="M17" s="1" t="s">
+      <c r="L17" t="s">
+        <v>215</v>
+      </c>
+      <c r="M17" t="s">
         <v>128</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="O17" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2678,31 +2840,31 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18">
-        <v>-247.5</v>
+        <v>-246.2</v>
       </c>
       <c r="F18">
-        <v>11.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G18">
-        <v>405</v>
+        <v>233</v>
       </c>
       <c r="H18">
-        <v>-50</v>
+        <v>-60.6</v>
       </c>
       <c r="I18">
-        <v>0.61</v>
+        <v>0.31</v>
       </c>
       <c r="J18">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="K18" t="s">
         <v>122</v>
@@ -2711,13 +2873,13 @@
         <v>210</v>
       </c>
       <c r="M18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="O18" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2725,34 +2887,34 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E19">
-        <v>-239.1</v>
+        <v>-230.6</v>
       </c>
       <c r="F19">
-        <v>9.27</v>
+        <v>13.56</v>
       </c>
       <c r="G19">
-        <v>365</v>
-      </c>
-      <c r="H19">
-        <v>-63</v>
-      </c>
-      <c r="I19">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="J19">
+        <v>1000</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-67</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J19" s="1">
         <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L19" t="s">
         <v>210</v>
@@ -2761,39 +2923,39 @@
         <v>127</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="O19" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="1">
-        <v>-250.3</v>
-      </c>
-      <c r="F20" s="1">
-        <v>20</v>
-      </c>
-      <c r="G20" s="1">
-        <v>68.599999999999994</v>
+        <v>106</v>
+      </c>
+      <c r="E20">
+        <v>-250</v>
+      </c>
+      <c r="F20">
+        <v>17.2</v>
+      </c>
+      <c r="G20">
+        <v>77</v>
       </c>
       <c r="H20">
-        <v>-58.2</v>
+        <v>-71.900000000000006</v>
       </c>
       <c r="I20">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
       <c r="J20">
         <v>28</v>
@@ -2808,10 +2970,10 @@
         <v>128</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="O20" t="s">
-        <v>157</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2819,46 +2981,46 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21">
-        <v>-242.6</v>
+        <v>-251.7</v>
       </c>
       <c r="F21">
-        <v>15.67</v>
+        <v>20</v>
       </c>
       <c r="G21">
-        <v>188</v>
-      </c>
-      <c r="H21">
-        <v>-59</v>
-      </c>
-      <c r="I21">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="J21">
-        <v>65</v>
+        <v>59.78</v>
+      </c>
+      <c r="H21" s="1">
+        <v>-58.7</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J21" s="1">
+        <v>28</v>
       </c>
       <c r="K21" t="s">
         <v>122</v>
       </c>
       <c r="L21" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="O21" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2866,46 +3028,46 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E22">
-        <v>-247</v>
+        <v>-250.6</v>
       </c>
       <c r="F22">
-        <v>1.1499999999999999</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="G22">
-        <v>414</v>
+        <v>135</v>
       </c>
       <c r="H22">
-        <v>-49</v>
+        <v>-57</v>
       </c>
       <c r="I22">
-        <v>0.24</v>
+        <v>0.38</v>
       </c>
       <c r="J22">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="K22" t="s">
-        <v>122</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="M22" t="s">
         <v>128</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="O22" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2913,31 +3075,31 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E23">
-        <v>-248.1</v>
+        <v>-249.4</v>
       </c>
       <c r="F23">
-        <v>9.1999999999999993</v>
+        <v>3.5</v>
       </c>
       <c r="G23">
-        <v>101</v>
-      </c>
-      <c r="H23">
-        <v>-56</v>
-      </c>
-      <c r="I23">
-        <v>0.27</v>
-      </c>
-      <c r="J23">
-        <v>130</v>
+        <v>182</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-59</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="J23" s="1">
+        <v>40</v>
       </c>
       <c r="K23" t="s">
         <v>122</v>
@@ -2949,86 +3111,86 @@
         <v>128</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="O23" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E24">
-        <v>-239</v>
+        <v>-248.7</v>
       </c>
       <c r="F24">
-        <v>21.7</v>
+        <v>36</v>
       </c>
       <c r="G24">
-        <v>240</v>
+        <v>72</v>
       </c>
       <c r="H24">
-        <v>-50</v>
+        <v>-59.7</v>
       </c>
       <c r="I24">
-        <v>0.17</v>
+        <v>0.47</v>
       </c>
       <c r="J24">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K24" t="s">
         <v>122</v>
       </c>
       <c r="L24" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M24" t="s">
         <v>128</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="O24" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25">
-        <v>-250.6</v>
-      </c>
-      <c r="F25">
-        <v>19.8</v>
-      </c>
-      <c r="G25">
-        <v>66.2</v>
+        <v>107</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-251.5</v>
+      </c>
+      <c r="F25" s="1">
+        <v>10.8</v>
+      </c>
+      <c r="G25" s="1">
+        <v>79.7</v>
       </c>
       <c r="H25">
-        <v>-61</v>
+        <v>-51.1</v>
       </c>
       <c r="I25">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="J25">
         <v>28</v>
@@ -3043,10 +3205,10 @@
         <v>128</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="O25" t="s">
-        <v>170</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3054,28 +3216,28 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="E26">
-        <v>-243.2</v>
+        <v>-224.8</v>
       </c>
       <c r="F26">
-        <v>2.5</v>
+        <v>11.95</v>
       </c>
       <c r="G26">
-        <v>397</v>
+        <v>1670</v>
       </c>
       <c r="H26">
-        <v>-54.8</v>
+        <v>-52</v>
       </c>
       <c r="I26">
-        <v>2.75E-2</v>
+        <v>0.18</v>
       </c>
       <c r="J26">
         <v>65</v>
@@ -3090,10 +3252,10 @@
         <v>127</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="O26" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3101,46 +3263,46 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>177</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="E27">
-        <v>-239.2</v>
+        <v>-242.3</v>
       </c>
       <c r="F27">
-        <v>1.6</v>
+        <v>3.25</v>
       </c>
       <c r="G27">
-        <v>860</v>
-      </c>
-      <c r="H27">
-        <v>-57</v>
+        <v>428</v>
+      </c>
+      <c r="H27" s="1">
+        <v>-55</v>
       </c>
       <c r="I27">
-        <v>0.33</v>
-      </c>
-      <c r="J27">
-        <v>28</v>
-      </c>
-      <c r="K27" t="s">
+        <v>0.39</v>
+      </c>
+      <c r="J27" s="1">
+        <v>40</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="1" t="s">
         <v>128</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="O27" t="s">
-        <v>180</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3148,46 +3310,46 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="E28">
-        <v>-237</v>
+        <v>-247.5</v>
       </c>
       <c r="F28">
-        <v>10.7</v>
+        <v>11.7</v>
       </c>
       <c r="G28">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="H28">
-        <v>-42</v>
+        <v>-50</v>
       </c>
       <c r="I28">
-        <v>0.5</v>
+        <v>0.61</v>
       </c>
       <c r="J28">
-        <v>40</v>
-      </c>
-      <c r="K28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
         <v>122</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="L28" t="s">
         <v>210</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>128</v>
+      <c r="M28" t="s">
+        <v>127</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>184</v>
+        <v>46</v>
       </c>
       <c r="O28" t="s">
-        <v>185</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3195,28 +3357,28 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29">
-        <v>-230</v>
+        <v>-239.1</v>
       </c>
       <c r="F29">
-        <v>20.9</v>
+        <v>9.27</v>
       </c>
       <c r="G29">
-        <v>557</v>
+        <v>365</v>
       </c>
       <c r="H29">
-        <v>-73.7</v>
+        <v>-63</v>
       </c>
       <c r="I29">
-        <v>0.77</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="J29">
         <v>65</v>
@@ -3228,60 +3390,60 @@
         <v>210</v>
       </c>
       <c r="M29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="O29" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30">
-        <v>-238.3</v>
-      </c>
-      <c r="F30">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="G30">
-        <v>390</v>
+        <v>107</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-250.3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>20</v>
+      </c>
+      <c r="G30" s="1">
+        <v>68.599999999999994</v>
       </c>
       <c r="H30">
-        <v>-41</v>
+        <v>-58.2</v>
       </c>
       <c r="I30">
-        <v>0.38</v>
+        <v>0.23</v>
       </c>
       <c r="J30">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="K30" t="s">
         <v>122</v>
       </c>
       <c r="L30" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M30" t="s">
         <v>128</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="O30" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3289,46 +3451,46 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31">
+        <v>-242.6</v>
+      </c>
+      <c r="F31">
+        <v>15.67</v>
+      </c>
+      <c r="G31">
+        <v>188</v>
+      </c>
+      <c r="H31">
+        <v>-59</v>
+      </c>
+      <c r="I31">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="J31">
         <v>65</v>
-      </c>
-      <c r="D31" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31">
-        <v>-249.8</v>
-      </c>
-      <c r="F31">
-        <v>16.7</v>
-      </c>
-      <c r="G31">
-        <v>79.3</v>
-      </c>
-      <c r="H31">
-        <v>-63.6</v>
-      </c>
-      <c r="I31">
-        <v>0.22</v>
-      </c>
-      <c r="J31">
-        <v>28</v>
       </c>
       <c r="K31" t="s">
         <v>122</v>
       </c>
       <c r="L31" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="O31" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3336,46 +3498,46 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E32">
-        <v>-250.5</v>
+        <v>-247</v>
       </c>
       <c r="F32">
-        <v>15.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G32">
-        <v>76</v>
+        <v>414</v>
       </c>
       <c r="H32">
-        <v>-65</v>
+        <v>-49</v>
       </c>
       <c r="I32">
-        <v>0.17</v>
+        <v>0.24</v>
       </c>
       <c r="J32">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K32" t="s">
         <v>122</v>
       </c>
       <c r="L32" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M32" t="s">
         <v>128</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="O32" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3383,46 +3545,46 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>187</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E33">
-        <v>-248</v>
+        <v>-248.1</v>
       </c>
       <c r="F33">
-        <v>21</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G33">
-        <v>87.1</v>
+        <v>101</v>
       </c>
       <c r="H33">
-        <v>-53.7</v>
+        <v>-56</v>
       </c>
       <c r="I33">
-        <v>0.34</v>
+        <v>0.27</v>
       </c>
       <c r="J33">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="K33" t="s">
         <v>122</v>
       </c>
       <c r="L33" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M33" t="s">
         <v>128</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>188</v>
+        <v>54</v>
       </c>
       <c r="O33" t="s">
-        <v>189</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3430,46 +3592,46 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E34">
-        <v>-250.6</v>
+        <v>-239</v>
       </c>
       <c r="F34">
-        <v>17.899999999999999</v>
+        <v>21.7</v>
       </c>
       <c r="G34">
-        <v>77.099999999999994</v>
+        <v>240</v>
       </c>
       <c r="H34">
-        <v>-60.3</v>
+        <v>-50</v>
       </c>
       <c r="I34">
-        <v>0.36</v>
+        <v>0.17</v>
       </c>
       <c r="J34">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K34" t="s">
         <v>122</v>
       </c>
       <c r="L34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M34" t="s">
         <v>128</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="O34" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3477,28 +3639,28 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="E35">
-        <v>-251.7</v>
+        <v>-250.6</v>
       </c>
       <c r="F35">
-        <v>10.8</v>
+        <v>19.8</v>
       </c>
       <c r="G35">
-        <v>107.6</v>
+        <v>66.2</v>
       </c>
       <c r="H35">
-        <v>-50.4</v>
+        <v>-61</v>
       </c>
       <c r="I35">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="J35">
         <v>28</v>
@@ -3513,10 +3675,10 @@
         <v>128</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="O35" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3524,34 +3686,34 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="E36">
-        <v>-233.8</v>
+        <v>-243.2</v>
       </c>
       <c r="F36">
-        <v>9.8800000000000008</v>
+        <v>2.5</v>
       </c>
       <c r="G36">
-        <v>648</v>
+        <v>397</v>
       </c>
       <c r="H36">
-        <v>-58</v>
+        <v>-54.8</v>
       </c>
       <c r="I36">
-        <v>0.108</v>
+        <v>2.75E-2</v>
       </c>
       <c r="J36">
         <v>65</v>
       </c>
       <c r="K36" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L36" t="s">
         <v>210</v>
@@ -3560,51 +3722,531 @@
         <v>127</v>
       </c>
       <c r="N36" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37">
+        <v>-239.2</v>
+      </c>
+      <c r="F37">
+        <v>1.6</v>
+      </c>
+      <c r="G37">
+        <v>860</v>
+      </c>
+      <c r="H37">
+        <v>-57</v>
+      </c>
+      <c r="I37">
+        <v>0.33</v>
+      </c>
+      <c r="J37">
+        <v>28</v>
+      </c>
+      <c r="K37" t="s">
+        <v>122</v>
+      </c>
+      <c r="L37" t="s">
+        <v>210</v>
+      </c>
+      <c r="M37" t="s">
+        <v>128</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="O37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E38">
+        <v>-237</v>
+      </c>
+      <c r="F38">
+        <v>10.7</v>
+      </c>
+      <c r="G38">
+        <v>420</v>
+      </c>
+      <c r="H38">
+        <v>-42</v>
+      </c>
+      <c r="I38">
+        <v>0.5</v>
+      </c>
+      <c r="J38">
+        <v>40</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39">
+        <v>-230</v>
+      </c>
+      <c r="F39">
+        <v>20.9</v>
+      </c>
+      <c r="G39">
+        <v>557</v>
+      </c>
+      <c r="H39">
+        <v>-73.7</v>
+      </c>
+      <c r="I39">
+        <v>0.77</v>
+      </c>
+      <c r="J39">
+        <v>65</v>
+      </c>
+      <c r="K39" t="s">
+        <v>122</v>
+      </c>
+      <c r="L39" t="s">
+        <v>210</v>
+      </c>
+      <c r="M39" t="s">
+        <v>128</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40">
+        <v>-238.3</v>
+      </c>
+      <c r="F40">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G40">
+        <v>390</v>
+      </c>
+      <c r="H40">
+        <v>-41</v>
+      </c>
+      <c r="I40">
+        <v>0.38</v>
+      </c>
+      <c r="J40">
+        <v>65</v>
+      </c>
+      <c r="K40" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" t="s">
+        <v>210</v>
+      </c>
+      <c r="M40" t="s">
+        <v>128</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41">
+        <v>-249.8</v>
+      </c>
+      <c r="F41">
+        <v>16.7</v>
+      </c>
+      <c r="G41">
+        <v>79.3</v>
+      </c>
+      <c r="H41">
+        <v>-63.6</v>
+      </c>
+      <c r="I41">
+        <v>0.22</v>
+      </c>
+      <c r="J41">
+        <v>28</v>
+      </c>
+      <c r="K41" t="s">
+        <v>122</v>
+      </c>
+      <c r="L41" t="s">
+        <v>213</v>
+      </c>
+      <c r="M41" t="s">
+        <v>128</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42">
+        <v>-250.5</v>
+      </c>
+      <c r="F42">
+        <v>15.3</v>
+      </c>
+      <c r="G42">
+        <v>76</v>
+      </c>
+      <c r="H42">
+        <v>-65</v>
+      </c>
+      <c r="I42">
+        <v>0.17</v>
+      </c>
+      <c r="J42">
+        <v>40</v>
+      </c>
+      <c r="K42" t="s">
+        <v>122</v>
+      </c>
+      <c r="L42" t="s">
+        <v>215</v>
+      </c>
+      <c r="M42" t="s">
+        <v>128</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E43">
+        <v>-248</v>
+      </c>
+      <c r="F43">
+        <v>21</v>
+      </c>
+      <c r="G43">
+        <v>87.1</v>
+      </c>
+      <c r="H43">
+        <v>-53.7</v>
+      </c>
+      <c r="I43">
+        <v>0.34</v>
+      </c>
+      <c r="J43">
+        <v>28</v>
+      </c>
+      <c r="K43" t="s">
+        <v>122</v>
+      </c>
+      <c r="L43" t="s">
+        <v>213</v>
+      </c>
+      <c r="M43" t="s">
+        <v>128</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44">
+        <v>-250.6</v>
+      </c>
+      <c r="F44">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G44">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="H44">
+        <v>-60.3</v>
+      </c>
+      <c r="I44">
+        <v>0.36</v>
+      </c>
+      <c r="J44">
+        <v>28</v>
+      </c>
+      <c r="K44" t="s">
+        <v>122</v>
+      </c>
+      <c r="L44" t="s">
+        <v>213</v>
+      </c>
+      <c r="M44" t="s">
+        <v>128</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="b">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>198</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45">
+        <v>-251.7</v>
+      </c>
+      <c r="F45">
+        <v>10.8</v>
+      </c>
+      <c r="G45">
+        <v>107.6</v>
+      </c>
+      <c r="H45">
+        <v>-50.4</v>
+      </c>
+      <c r="I45">
+        <v>0.21</v>
+      </c>
+      <c r="J45">
+        <v>28</v>
+      </c>
+      <c r="K45" t="s">
+        <v>122</v>
+      </c>
+      <c r="L45" t="s">
+        <v>213</v>
+      </c>
+      <c r="M45" t="s">
+        <v>128</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O45" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46">
+        <v>-233.8</v>
+      </c>
+      <c r="F46">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="G46">
+        <v>648</v>
+      </c>
+      <c r="H46">
+        <v>-58</v>
+      </c>
+      <c r="I46">
+        <v>0.108</v>
+      </c>
+      <c r="J46">
+        <v>65</v>
+      </c>
+      <c r="K46" t="s">
+        <v>122</v>
+      </c>
+      <c r="L46" t="s">
+        <v>210</v>
+      </c>
+      <c r="M46" t="s">
+        <v>127</v>
+      </c>
+      <c r="N46" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O46" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" xr:uid="{E232B5B4-E744-4E0B-B74E-3A04EF1AEFB3}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{0552F544-F0DF-4D55-8249-04CEAD860409}"/>
-    <hyperlink ref="N36" r:id="rId3" xr:uid="{55C109CE-5924-4938-84F7-DC204AAF8498}"/>
-    <hyperlink ref="N35" r:id="rId4" xr:uid="{3B969C18-0841-400E-8B75-7DAFC84A97CA}"/>
-    <hyperlink ref="N34" r:id="rId5" xr:uid="{18C51F5D-A33C-401D-AB3E-A63671D0A04A}"/>
-    <hyperlink ref="N33" r:id="rId6" xr:uid="{D7E1F942-4441-4747-A77E-732FDFD2599A}"/>
-    <hyperlink ref="N32" r:id="rId7" xr:uid="{028A896E-079E-49D9-836C-8D977A498D2D}"/>
-    <hyperlink ref="N31" r:id="rId8" xr:uid="{53C48B87-16DD-4255-B3D5-436CB6FC1B5A}"/>
-    <hyperlink ref="N30" r:id="rId9" xr:uid="{8DFB28FC-7A01-49A8-AC0B-170F9DEAAAB4}"/>
-    <hyperlink ref="N29" r:id="rId10" xr:uid="{26C50D4D-B39A-4BEE-8922-8A7309EF0292}"/>
-    <hyperlink ref="N28" r:id="rId11" xr:uid="{E69BF196-16B7-4364-903A-2123B43A87A3}"/>
-    <hyperlink ref="N27" r:id="rId12" xr:uid="{C41406A6-917F-4E8D-B390-4332AFB727AB}"/>
-    <hyperlink ref="N26" r:id="rId13" xr:uid="{4510B694-D5FC-4DB3-861B-F3793CF682D9}"/>
-    <hyperlink ref="N25" r:id="rId14" xr:uid="{C5C68201-E1F1-4EB5-9D92-075C7CE22A2E}"/>
-    <hyperlink ref="N24" r:id="rId15" xr:uid="{678EE13B-2A37-46E2-A947-E4B14D73BFBE}"/>
-    <hyperlink ref="N23" r:id="rId16" xr:uid="{A8FBD716-533C-4303-86BF-F3C388B7B070}"/>
-    <hyperlink ref="N22" r:id="rId17" xr:uid="{97DA02D1-A5F4-49B1-B4DC-ACBA8E50454A}"/>
-    <hyperlink ref="N21" r:id="rId18" xr:uid="{8DFEAF18-73B3-4E4A-924B-3BEBB5BBE098}"/>
-    <hyperlink ref="N20" r:id="rId19" xr:uid="{ED849692-445E-485A-8CFA-C96333C6829E}"/>
-    <hyperlink ref="N19" r:id="rId20" xr:uid="{0D9C2A66-F9CA-43AC-AB7D-D71CF2D8B664}"/>
-    <hyperlink ref="N18" r:id="rId21" xr:uid="{0CFBD616-FE63-45C3-A5CF-65E0685A27D2}"/>
-    <hyperlink ref="N17" r:id="rId22" xr:uid="{26D68220-1314-4C15-A8BD-E0882DF8DB5B}"/>
-    <hyperlink ref="N16" r:id="rId23" xr:uid="{992A3000-449E-4B9B-BA03-B2A2790EEECC}"/>
-    <hyperlink ref="N15" r:id="rId24" xr:uid="{22A3DEE5-CCD3-4CFC-BA6C-E0E5BC1CFBC5}"/>
-    <hyperlink ref="N14" r:id="rId25" xr:uid="{308D753C-BE30-444C-A951-A9F9A6C229B7}"/>
-    <hyperlink ref="N13" r:id="rId26" xr:uid="{714B659D-D4AF-46E2-91E7-5661F823920C}"/>
-    <hyperlink ref="N12" r:id="rId27" xr:uid="{7A34D073-296E-4228-B6F9-7D19F31A3C46}"/>
-    <hyperlink ref="N11" r:id="rId28" xr:uid="{5ABA6C2A-E0D9-43F1-8C30-427ABD013790}"/>
-    <hyperlink ref="N10" r:id="rId29" xr:uid="{56C8C4C6-94D9-4798-9BCC-875966148F14}"/>
-    <hyperlink ref="N9" r:id="rId30" xr:uid="{A3D85411-0B02-49B0-A94A-1431B7EA57E2}"/>
-    <hyperlink ref="N8" r:id="rId31" xr:uid="{6685A9BE-E8A9-46B7-8259-89DEE2AB0A56}"/>
-    <hyperlink ref="N7" r:id="rId32" xr:uid="{CC7442BF-8449-47F3-B83F-F07DC77C8B69}"/>
-    <hyperlink ref="N6" r:id="rId33" xr:uid="{585670AC-1996-48D5-8CEB-C132C62B805F}"/>
-    <hyperlink ref="N5" r:id="rId34" xr:uid="{646F44DE-6CBC-4EF5-B333-1D33428DAB24}"/>
+    <hyperlink ref="N16" r:id="rId1" xr:uid="{E232B5B4-E744-4E0B-B74E-3A04EF1AEFB3}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{0552F544-F0DF-4D55-8249-04CEAD860409}"/>
+    <hyperlink ref="N46" r:id="rId3" xr:uid="{55C109CE-5924-4938-84F7-DC204AAF8498}"/>
+    <hyperlink ref="N45" r:id="rId4" xr:uid="{3B969C18-0841-400E-8B75-7DAFC84A97CA}"/>
+    <hyperlink ref="N44" r:id="rId5" xr:uid="{18C51F5D-A33C-401D-AB3E-A63671D0A04A}"/>
+    <hyperlink ref="N43" r:id="rId6" xr:uid="{D7E1F942-4441-4747-A77E-732FDFD2599A}"/>
+    <hyperlink ref="N42" r:id="rId7" xr:uid="{028A896E-079E-49D9-836C-8D977A498D2D}"/>
+    <hyperlink ref="N41" r:id="rId8" xr:uid="{53C48B87-16DD-4255-B3D5-436CB6FC1B5A}"/>
+    <hyperlink ref="N40" r:id="rId9" xr:uid="{8DFB28FC-7A01-49A8-AC0B-170F9DEAAAB4}"/>
+    <hyperlink ref="N39" r:id="rId10" xr:uid="{26C50D4D-B39A-4BEE-8922-8A7309EF0292}"/>
+    <hyperlink ref="N38" r:id="rId11" xr:uid="{E69BF196-16B7-4364-903A-2123B43A87A3}"/>
+    <hyperlink ref="N37" r:id="rId12" xr:uid="{C41406A6-917F-4E8D-B390-4332AFB727AB}"/>
+    <hyperlink ref="N36" r:id="rId13" xr:uid="{4510B694-D5FC-4DB3-861B-F3793CF682D9}"/>
+    <hyperlink ref="N35" r:id="rId14" xr:uid="{C5C68201-E1F1-4EB5-9D92-075C7CE22A2E}"/>
+    <hyperlink ref="N34" r:id="rId15" xr:uid="{678EE13B-2A37-46E2-A947-E4B14D73BFBE}"/>
+    <hyperlink ref="N33" r:id="rId16" xr:uid="{A8FBD716-533C-4303-86BF-F3C388B7B070}"/>
+    <hyperlink ref="N32" r:id="rId17" xr:uid="{97DA02D1-A5F4-49B1-B4DC-ACBA8E50454A}"/>
+    <hyperlink ref="N31" r:id="rId18" xr:uid="{8DFEAF18-73B3-4E4A-924B-3BEBB5BBE098}"/>
+    <hyperlink ref="N30" r:id="rId19" xr:uid="{ED849692-445E-485A-8CFA-C96333C6829E}"/>
+    <hyperlink ref="N29" r:id="rId20" xr:uid="{0D9C2A66-F9CA-43AC-AB7D-D71CF2D8B664}"/>
+    <hyperlink ref="N28" r:id="rId21" xr:uid="{0CFBD616-FE63-45C3-A5CF-65E0685A27D2}"/>
+    <hyperlink ref="N27" r:id="rId22" xr:uid="{26D68220-1314-4C15-A8BD-E0882DF8DB5B}"/>
+    <hyperlink ref="N26" r:id="rId23" xr:uid="{992A3000-449E-4B9B-BA03-B2A2790EEECC}"/>
+    <hyperlink ref="N25" r:id="rId24" xr:uid="{22A3DEE5-CCD3-4CFC-BA6C-E0E5BC1CFBC5}"/>
+    <hyperlink ref="N24" r:id="rId25" xr:uid="{308D753C-BE30-444C-A951-A9F9A6C229B7}"/>
+    <hyperlink ref="N23" r:id="rId26" xr:uid="{714B659D-D4AF-46E2-91E7-5661F823920C}"/>
+    <hyperlink ref="N22" r:id="rId27" xr:uid="{7A34D073-296E-4228-B6F9-7D19F31A3C46}"/>
+    <hyperlink ref="N21" r:id="rId28" xr:uid="{5ABA6C2A-E0D9-43F1-8C30-427ABD013790}"/>
+    <hyperlink ref="N20" r:id="rId29" xr:uid="{56C8C4C6-94D9-4798-9BCC-875966148F14}"/>
+    <hyperlink ref="N19" r:id="rId30" xr:uid="{A3D85411-0B02-49B0-A94A-1431B7EA57E2}"/>
+    <hyperlink ref="N18" r:id="rId31" xr:uid="{6685A9BE-E8A9-46B7-8259-89DEE2AB0A56}"/>
+    <hyperlink ref="N4" r:id="rId32" xr:uid="{CC7442BF-8449-47F3-B83F-F07DC77C8B69}"/>
+    <hyperlink ref="N11" r:id="rId33" xr:uid="{585670AC-1996-48D5-8CEB-C132C62B805F}"/>
+    <hyperlink ref="N17" r:id="rId34" xr:uid="{646F44DE-6CBC-4EF5-B333-1D33428DAB24}"/>
+    <hyperlink ref="N5" r:id="rId35" xr:uid="{A6BE4BF7-1D5A-46F1-A4B4-9721E669A4A3}"/>
+    <hyperlink ref="N6" r:id="rId36" xr:uid="{5269EBCA-52F1-4FA7-A50D-BF695A6A04A9}"/>
+    <hyperlink ref="N7" r:id="rId37" xr:uid="{F1E9804B-4C92-4798-A8CF-2869EC5B79F1}"/>
+    <hyperlink ref="N8" r:id="rId38" xr:uid="{10F5E133-83B9-4E7C-B918-32C91FD49F2F}"/>
+    <hyperlink ref="N9" r:id="rId39" xr:uid="{D912F49A-B32B-4A83-8641-5748C46F9A7F}"/>
+    <hyperlink ref="N10" r:id="rId40" xr:uid="{B8FB1BDC-6E48-4899-9CE0-0F6ACB1E44EC}"/>
+    <hyperlink ref="N12" r:id="rId41" xr:uid="{9E139979-0BD2-490F-B51D-2BCFDC67DC94}"/>
+    <hyperlink ref="N13" r:id="rId42" xr:uid="{B21FBA00-0C83-4925-A35B-52DB494E3481}"/>
+    <hyperlink ref="N14" r:id="rId43" xr:uid="{D06194B6-BF8A-4457-9006-3D7B0B24DDD6}"/>
+    <hyperlink ref="N15" r:id="rId44" xr:uid="{9471A842-C955-4CC7-A07A-56B6F7B13293}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
 

</xml_diff>